<commit_message>
aid improved animated plot
</commit_message>
<xml_diff>
--- a/data_raw/world_aid_timeline.xlsx
+++ b/data_raw/world_aid_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\EMSE 4572\Proposals\proj1\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59500A77-95BB-4737-9C74-FA1A847A73A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31407F94-6C1F-4E8C-BCB4-B4FD583AC997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>Backpack</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>GCS-200 de-mining vehicle</t>
+  </si>
+  <si>
+    <t>Bandvagn 206 ATV</t>
+  </si>
+  <si>
+    <t>Wisent mine-clearing tank</t>
+  </si>
+  <si>
+    <t>VECTOR drone spare parts package</t>
+  </si>
+  <si>
+    <t>Cryptophone (encrypted sat phone)</t>
+  </si>
+  <si>
+    <t>40mm rounds</t>
+  </si>
+  <si>
+    <t>1202 infusion kits</t>
   </si>
 </sst>
 </file>
@@ -502,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F42"/>
+  <dimension ref="B2:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1197,6 +1221,227 @@
         <v>27477</v>
       </c>
     </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="2">
+        <v>45203</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54">
+        <v>32823</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>